<commit_message>
Run job commit message
</commit_message>
<xml_diff>
--- a/JT_RETURN_DAMAGE_ANALYSIS_SCRIPT_TABLE.xlsx
+++ b/JT_RETURN_DAMAGE_ANALYSIS_SCRIPT_TABLE.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="115">
   <si>
     <t>JOB_GROUP</t>
   </si>
@@ -71,10 +71,10 @@
     <t>use warehouse demo_WH;</t>
   </si>
   <si>
-    <t>2021-05-12 12:57:52.186</t>
-  </si>
-  <si>
-    <t>2021-05-12 12:57:55.663</t>
+    <t>2021-09-02 09:42:06.992</t>
+  </si>
+  <si>
+    <t>2021-09-02 09:42:08.805</t>
   </si>
   <si>
     <t/>
@@ -86,10 +86,10 @@
     <t>use database Demo1_DB;</t>
   </si>
   <si>
-    <t>2021-05-12 12:57:56.742</t>
-  </si>
-  <si>
-    <t>2021-05-12 12:57:59.426</t>
+    <t>2021-09-02 09:42:09.228</t>
+  </si>
+  <si>
+    <t>2021-09-02 09:42:10.947</t>
   </si>
   <si>
     <t>5</t>
@@ -104,10 +104,10 @@
     <t>create or replace table ETL_SALES_TABLE_1 (Product_Id Integer, Transaction_Id string,Return_date date,Region string,Zip_code integer,Items_Sold Integer,Items_Returned Integer, Reason string,Unit_Price Integer,Sale_Amount Integer,Return_Amount Integer,Month_of_Return Integer,Corrected_Revenue Integer);</t>
   </si>
   <si>
-    <t>2021-05-12 12:58:00.18</t>
-  </si>
-  <si>
-    <t>2021-05-12 12:58:03.059</t>
+    <t>2021-09-02 09:42:11.367</t>
+  </si>
+  <si>
+    <t>2021-09-02 09:42:13.491</t>
   </si>
   <si>
     <t>7</t>
@@ -116,10 +116,10 @@
     <t>Insert Into ETL_SALES_TABLE_1 (Region) Values ('T1 -- ORIGINAL' );</t>
   </si>
   <si>
-    <t>2021-05-12 12:58:03.901</t>
-  </si>
-  <si>
-    <t>2021-05-12 12:58:07.231</t>
+    <t>2021-09-02 09:42:13.872</t>
+  </si>
+  <si>
+    <t>2021-09-02 09:42:14.847</t>
   </si>
   <si>
     <t>8</t>
@@ -143,10 +143,10 @@
     <t>copy into ETL_SALES_TABLE_1(Product_Id, Transaction_Id, Return_date, Region, Zip_code, Items_Sold, Items_Returned, Reason, Unit_Price) from (select t.$1, t.$2, t.$3, t.$4, t.$5, t.$6, t.$7, t.$8, t.$9 from @demo_s3_stage/Sales-demo-data.csv t) file_format = (type = csv field_delimiter = ',' skip_header = 1);</t>
   </si>
   <si>
-    <t>2021-05-12 12:58:08.236</t>
-  </si>
-  <si>
-    <t>2021-05-12 12:58:12.47</t>
+    <t>2021-09-02 09:42:15.132</t>
+  </si>
+  <si>
+    <t>2021-09-02 09:42:18.079</t>
   </si>
   <si>
     <t>11</t>
@@ -167,10 +167,10 @@
     <t>CREATE OR REPLACE TABLE ETL_SALES_TABLE_2 like ETL_SALES_TABLE_1;</t>
   </si>
   <si>
-    <t>2021-05-12 12:58:13.187</t>
-  </si>
-  <si>
-    <t>2021-05-12 12:58:16.303</t>
+    <t>2021-09-02 09:42:18.443</t>
+  </si>
+  <si>
+    <t>2021-09-02 09:42:20.197</t>
   </si>
   <si>
     <t>14</t>
@@ -179,10 +179,10 @@
     <t>Insert Into ETL_SALES_TABLE_2 (Region) Values ('T2-ETL Table' );</t>
   </si>
   <si>
-    <t>2021-05-12 12:58:17.103</t>
-  </si>
-  <si>
-    <t>2021-05-12 12:58:21.402</t>
+    <t>2021-09-02 09:42:20.473</t>
+  </si>
+  <si>
+    <t>2021-09-02 09:42:21.365</t>
   </si>
   <si>
     <t>15</t>
@@ -191,10 +191,10 @@
     <t>insert into ETL_SALES_TABLE_2 select * from ETL_SALES_TABLE_1 where Reason ='Damaged';</t>
   </si>
   <si>
-    <t>2021-05-12 12:58:22.106</t>
-  </si>
-  <si>
-    <t>2021-05-12 12:58:24.89</t>
+    <t>2021-09-02 09:42:21.635</t>
+  </si>
+  <si>
+    <t>2021-09-02 09:42:23.068</t>
   </si>
   <si>
     <t>16</t>
@@ -209,10 +209,10 @@
     <t>CREATE OR REPLACE TABLE ETL_SALES_TABLE_3 CLONE ETL_SALES_TABLE_2;</t>
   </si>
   <si>
-    <t>2021-05-12 12:58:26.056</t>
-  </si>
-  <si>
-    <t>2021-05-12 12:58:29.622</t>
+    <t>2021-09-02 09:42:23.374</t>
+  </si>
+  <si>
+    <t>2021-09-02 09:42:25.889</t>
   </si>
   <si>
     <t>18</t>
@@ -221,10 +221,10 @@
     <t>Update ETL_SALES_TABLE_3 set Region='T3-Sale Amount Computed' where Region = 'T2-ETL Table';</t>
   </si>
   <si>
-    <t>2021-05-12 12:58:30.338</t>
-  </si>
-  <si>
-    <t>2021-05-12 12:58:33.402</t>
+    <t>2021-09-02 09:42:26.343</t>
+  </si>
+  <si>
+    <t>2021-09-02 09:42:27.42</t>
   </si>
   <si>
     <t>19</t>
@@ -233,10 +233,10 @@
     <t>Update ETL_SALES_TABLE_3 set SALE_AMOUNT=(Unit_Price*ITEMS_SOLD);</t>
   </si>
   <si>
-    <t>2021-05-12 12:58:34.236</t>
-  </si>
-  <si>
-    <t>2021-05-12 12:58:37.243</t>
+    <t>2021-09-02 09:42:27.831</t>
+  </si>
+  <si>
+    <t>2021-09-02 09:42:28.882</t>
   </si>
   <si>
     <t>20</t>
@@ -245,10 +245,10 @@
     <t>CREATE OR REPLACE TABLE ETL_SALES_TABLE_4 CLONE ETL_SALES_TABLE_3;</t>
   </si>
   <si>
-    <t>2021-05-12 12:58:37.885</t>
-  </si>
-  <si>
-    <t>2021-05-12 12:58:41.182</t>
+    <t>2021-09-02 09:42:29.265</t>
+  </si>
+  <si>
+    <t>2021-09-02 09:42:31.785</t>
   </si>
   <si>
     <t>21</t>
@@ -257,10 +257,10 @@
     <t>Update ETL_SALES_TABLE_4 set Region='T4-Return Amount Computed' where Region = 'T3-Sale Amount Computed';</t>
   </si>
   <si>
-    <t>2021-05-12 12:58:42.266</t>
-  </si>
-  <si>
-    <t>2021-05-12 12:58:44.997</t>
+    <t>2021-09-02 09:42:32.152</t>
+  </si>
+  <si>
+    <t>2021-09-02 09:42:33.169</t>
   </si>
   <si>
     <t>22</t>
@@ -269,10 +269,10 @@
     <t>Update ETL_SALES_TABLE_4 set RETURN_AMOUNT=(Unit_Price*ITEMS_RETURNED);</t>
   </si>
   <si>
-    <t>2021-05-12 12:58:45.656</t>
-  </si>
-  <si>
-    <t>2021-05-12 12:58:48.467</t>
+    <t>2021-09-02 09:42:33.531</t>
+  </si>
+  <si>
+    <t>2021-09-02 09:42:34.466</t>
   </si>
   <si>
     <t>23</t>
@@ -284,10 +284,7 @@
     <t>24</t>
   </si>
   <si>
-    <t>2021-05-12 12:58:49.187</t>
-  </si>
-  <si>
-    <t>2021-05-12 12:58:53.007</t>
+    <t>2021-09-02 09:42:34.819</t>
   </si>
   <si>
     <t>25</t>
@@ -1207,7 +1204,7 @@
         <v>90</v>
       </c>
       <c r="I25" t="s" s="2">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="J25" t="s" s="2">
         <v>21</v>
@@ -1218,10 +1215,10 @@
         <v>10</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C26" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26" t="s" s="2">
         <v>12</v>
@@ -1234,10 +1231,10 @@
       </c>
       <c r="G26" s="2"/>
       <c r="H26" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="I26" t="s" s="2">
         <v>93</v>
-      </c>
-      <c r="I26" t="s" s="2">
-        <v>94</v>
       </c>
       <c r="J26" t="s" s="2">
         <v>21</v>
@@ -1248,10 +1245,10 @@
         <v>10</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C27" t="s" s="2">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D27" t="s" s="2">
         <v>12</v>
@@ -1264,10 +1261,10 @@
       </c>
       <c r="G27" s="2"/>
       <c r="H27" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="I27" t="s" s="2">
         <v>96</v>
-      </c>
-      <c r="I27" t="s" s="2">
-        <v>97</v>
       </c>
       <c r="J27" t="s" s="2">
         <v>21</v>
@@ -1278,16 +1275,16 @@
         <v>10</v>
       </c>
       <c r="B28" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="C28" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="D28" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s" s="2">
         <v>98</v>
-      </c>
-      <c r="C28" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="D28" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="E28" t="s" s="2">
-        <v>99</v>
       </c>
       <c r="F28" t="s" s="2">
         <v>14</v>
@@ -1302,26 +1299,26 @@
         <v>10</v>
       </c>
       <c r="B29" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="C29" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="D29" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s" s="2">
         <v>100</v>
-      </c>
-      <c r="C29" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="D29" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="E29" t="s" s="2">
-        <v>101</v>
       </c>
       <c r="F29" t="s" s="2">
         <v>14</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="I29" t="s" s="2">
         <v>102</v>
-      </c>
-      <c r="I29" t="s" s="2">
-        <v>103</v>
       </c>
       <c r="J29" t="s" s="2">
         <v>21</v>
@@ -1332,26 +1329,26 @@
         <v>10</v>
       </c>
       <c r="B30" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="C30" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="D30" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s" s="2">
         <v>104</v>
-      </c>
-      <c r="C30" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="D30" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="E30" t="s" s="2">
-        <v>105</v>
       </c>
       <c r="F30" t="s" s="2">
         <v>14</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="I30" t="s" s="2">
         <v>106</v>
-      </c>
-      <c r="I30" t="s" s="2">
-        <v>107</v>
       </c>
       <c r="J30" t="s" s="2">
         <v>21</v>
@@ -1362,26 +1359,26 @@
         <v>10</v>
       </c>
       <c r="B31" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="C31" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="D31" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s" s="2">
         <v>108</v>
-      </c>
-      <c r="C31" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="D31" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="E31" t="s" s="2">
-        <v>109</v>
       </c>
       <c r="F31" t="s" s="2">
         <v>14</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="I31" t="s" s="2">
         <v>110</v>
-      </c>
-      <c r="I31" t="s" s="2">
-        <v>111</v>
       </c>
       <c r="J31" t="s" s="2">
         <v>21</v>
@@ -1392,27 +1389,27 @@
         <v>10</v>
       </c>
       <c r="B32" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="C32" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="D32" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s" s="2">
         <v>112</v>
-      </c>
-      <c r="C32" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="D32" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="E32" t="s" s="2">
-        <v>113</v>
       </c>
       <c r="F32" t="s" s="2">
         <v>14</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" t="s" s="2">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>